<commit_message>
WM analysis - markdown file
</commit_message>
<xml_diff>
--- a/data/20181122 WM tasks.xlsx
+++ b/data/20181122 WM tasks.xlsx
@@ -27,8 +27,8 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
-    <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4868" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4870" uniqueCount="575">
   <si>
     <t>Subject</t>
   </si>
@@ -1759,6 +1759,12 @@
   <si>
     <t>redundant_searches</t>
   </si>
+  <si>
+    <t>P1P2_first4</t>
+  </si>
+  <si>
+    <t>P1_first4</t>
+  </si>
 </sst>
 </file>
 
@@ -12750,7 +12756,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0">
@@ -12919,7 +12925,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="38">
     <pivotField axis="axisRow" showAll="0">
@@ -74248,12 +74254,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL121"/>
+  <dimension ref="A1:AN121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="AM26" sqref="AM26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74268,7 +74274,7 @@
     <col min="26" max="26" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -74383,8 +74389,14 @@
       <c r="AL1" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM1" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -74486,8 +74498,16 @@
         <f>IF(K2&lt;&gt;0, K2-AK2,"")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM2">
+        <f>O2+Q2+S2+U2+W2+Y2+2</f>
+        <v>4</v>
+      </c>
+      <c r="AN2">
+        <f>O2+S2+W2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
@@ -74595,8 +74615,16 @@
         <f>IF(K3&lt;&gt;0, K3-AK3,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM3">
+        <f t="shared" ref="AM3:AM66" si="1">O3+Q3+S3+U3+W3+Y3+2</f>
+        <v>4</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3:AN66" si="2">O3+S3+W3+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>37</v>
       </c>
@@ -74701,11 +74729,19 @@
         <v>6</v>
       </c>
       <c r="AL4">
-        <f t="shared" ref="AL4:AL43" si="1">IF(K4&lt;&gt;0, K4-AK4,"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ref="AL4:AL43" si="3">IF(K4&lt;&gt;0, K4-AK4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -74786,11 +74822,19 @@
         <v>7</v>
       </c>
       <c r="AL5">
+        <f t="shared" si="3"/>
+        <v>-6</v>
+      </c>
+      <c r="AM5">
         <f t="shared" si="1"/>
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -74895,11 +74939,19 @@
         <v>6</v>
       </c>
       <c r="AL6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AM6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
@@ -74998,11 +75050,19 @@
         <v>7</v>
       </c>
       <c r="AL7">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="AM7">
         <f t="shared" si="1"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
@@ -75107,11 +75167,19 @@
         <v>7</v>
       </c>
       <c r="AL8">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="AM8">
         <f t="shared" si="1"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -75193,11 +75261,19 @@
         <v>7</v>
       </c>
       <c r="AL9">
+        <f t="shared" si="3"/>
+        <v>-6</v>
+      </c>
+      <c r="AM9">
         <f t="shared" si="1"/>
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -75290,11 +75366,19 @@
         <v>8</v>
       </c>
       <c r="AL10">
+        <f t="shared" si="3"/>
+        <v>-6</v>
+      </c>
+      <c r="AM10">
         <f t="shared" si="1"/>
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
@@ -75399,11 +75483,19 @@
         <v>6</v>
       </c>
       <c r="AL11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AM11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -75505,11 +75597,19 @@
         <v>6</v>
       </c>
       <c r="AL12">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="AM12">
         <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -75608,11 +75708,19 @@
         <v>5</v>
       </c>
       <c r="AL13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM13">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
@@ -75699,11 +75807,19 @@
         <v>4</v>
       </c>
       <c r="AL14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM14">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -75808,11 +75924,19 @@
         <v>7</v>
       </c>
       <c r="AL15">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="AM15">
         <f t="shared" si="1"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -75893,11 +76017,19 @@
         <v>5</v>
       </c>
       <c r="AL16">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="AM16">
         <f t="shared" si="1"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -75996,11 +76128,19 @@
         <v>5</v>
       </c>
       <c r="AL17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM17">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN17">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
@@ -76087,11 +76227,19 @@
         <v>7</v>
       </c>
       <c r="AL18">
+        <f t="shared" si="3"/>
+        <v>-5</v>
+      </c>
+      <c r="AM18">
         <f t="shared" si="1"/>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -76196,11 +76344,19 @@
         <v>6</v>
       </c>
       <c r="AL19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AM19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>46</v>
       </c>
@@ -76305,11 +76461,19 @@
         <v>8</v>
       </c>
       <c r="AL20">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="AM20">
         <f t="shared" si="1"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
@@ -76414,11 +76578,19 @@
         <v>6</v>
       </c>
       <c r="AL21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AM21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN21">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -76511,11 +76683,19 @@
         <v>4</v>
       </c>
       <c r="AL22">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AM22">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN22">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
@@ -76608,11 +76788,19 @@
         <v>4</v>
       </c>
       <c r="AL23">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AM23">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
@@ -76711,11 +76899,19 @@
         <v>5</v>
       </c>
       <c r="AL24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM24">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN24">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>47</v>
       </c>
@@ -76814,11 +77010,19 @@
         <v>6</v>
       </c>
       <c r="AL25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AM25">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN25">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -76911,11 +77115,19 @@
         <v>4</v>
       </c>
       <c r="AL26">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AM26">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="AN26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>48</v>
       </c>
@@ -77002,11 +77214,19 @@
         <v>3</v>
       </c>
       <c r="AL27">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="AM27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AN27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>48</v>
       </c>
@@ -77093,11 +77313,19 @@
         <v>3</v>
       </c>
       <c r="AL28">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="AM28">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AN28">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>48</v>
       </c>
@@ -77184,11 +77412,19 @@
         <v>3</v>
       </c>
       <c r="AL29">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="AM29">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AN29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>49</v>
       </c>
@@ -77287,11 +77523,19 @@
         <v>5</v>
       </c>
       <c r="AL30">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM30">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN30">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>49</v>
       </c>
@@ -77390,11 +77634,19 @@
         <v>5</v>
       </c>
       <c r="AL31">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM31">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>49</v>
       </c>
@@ -77487,11 +77739,19 @@
         <v>4</v>
       </c>
       <c r="AL32">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AM32">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN32">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>49</v>
       </c>
@@ -77590,11 +77850,19 @@
         <v>5</v>
       </c>
       <c r="AL33">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM33">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN33">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
@@ -77687,11 +77955,19 @@
         <v>7</v>
       </c>
       <c r="AL34">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="AM34">
         <f t="shared" si="1"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN34">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>50</v>
       </c>
@@ -77784,11 +78060,19 @@
         <v>5</v>
       </c>
       <c r="AL35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM35">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN35">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>50</v>
       </c>
@@ -77893,11 +78177,19 @@
         <v>6</v>
       </c>
       <c r="AL36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AM36">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -77978,11 +78270,19 @@
         <v>6</v>
       </c>
       <c r="AL37">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="AM37">
         <f t="shared" si="1"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN37">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>52</v>
       </c>
@@ -78069,11 +78369,19 @@
         <v>7</v>
       </c>
       <c r="AL38">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="AM38">
         <f t="shared" si="1"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN38">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>52</v>
       </c>
@@ -78166,11 +78474,19 @@
         <v>6</v>
       </c>
       <c r="AL39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AM39">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN39">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>52</v>
       </c>
@@ -78269,11 +78585,19 @@
         <v>5</v>
       </c>
       <c r="AL40">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM40">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN40">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>52</v>
       </c>
@@ -78366,11 +78690,19 @@
         <v>4</v>
       </c>
       <c r="AL41">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AM41">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="AN41">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>53</v>
       </c>
@@ -78481,11 +78813,19 @@
         <v>8</v>
       </c>
       <c r="AL42">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="AM42">
         <f t="shared" si="1"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN42">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>53</v>
       </c>
@@ -78584,11 +78924,19 @@
         <v>5</v>
       </c>
       <c r="AL43">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM43">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN43">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>53</v>
       </c>
@@ -78693,11 +79041,19 @@
         <v>5</v>
       </c>
       <c r="AL44">
-        <f t="shared" ref="AL44:AL89" si="2">IF(K44&lt;&gt;0, K44-AK44,"")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ref="AL44:AL89" si="4">IF(K44&lt;&gt;0, K44-AK44,"")</f>
+        <v>1</v>
+      </c>
+      <c r="AM44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN44">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
@@ -78790,11 +79146,19 @@
         <v>4</v>
       </c>
       <c r="AL45">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AM45">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN45">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>102</v>
       </c>
@@ -78899,11 +79263,19 @@
         <v>6</v>
       </c>
       <c r="AL46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM46">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN46">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>102</v>
       </c>
@@ -79002,11 +79374,19 @@
         <v>6</v>
       </c>
       <c r="AL47">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM47">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN47">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>102</v>
       </c>
@@ -79105,11 +79485,19 @@
         <v>5</v>
       </c>
       <c r="AL48">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM48">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN48">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>102</v>
       </c>
@@ -79208,11 +79596,19 @@
         <v>5</v>
       </c>
       <c r="AL49">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM49">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN49">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>55</v>
       </c>
@@ -79311,11 +79707,19 @@
         <v>5</v>
       </c>
       <c r="AL50">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM50">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN50">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>55</v>
       </c>
@@ -79402,11 +79806,19 @@
         <v>6</v>
       </c>
       <c r="AL51">
+        <f t="shared" si="4"/>
+        <v>-3</v>
+      </c>
+      <c r="AM51">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="AN51">
         <f t="shared" si="2"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>55</v>
       </c>
@@ -79511,11 +79923,19 @@
         <v>6</v>
       </c>
       <c r="AL52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM52">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN52">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>55</v>
       </c>
@@ -79614,11 +80034,19 @@
         <v>5</v>
       </c>
       <c r="AL53">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM53">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN53">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>56</v>
       </c>
@@ -79711,11 +80139,19 @@
         <v>4</v>
       </c>
       <c r="AL54">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AM54">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN54">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>56</v>
       </c>
@@ -79808,11 +80244,19 @@
         <v>4</v>
       </c>
       <c r="AL55">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AM55">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AN55">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>56</v>
       </c>
@@ -79905,11 +80349,19 @@
         <v>4</v>
       </c>
       <c r="AL56">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AM56">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN56">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>56</v>
       </c>
@@ -80008,11 +80460,19 @@
         <v>5</v>
       </c>
       <c r="AL57">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM57">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN57">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -80117,11 +80577,19 @@
         <v>8</v>
       </c>
       <c r="AL58">
+        <f t="shared" si="4"/>
+        <v>-4</v>
+      </c>
+      <c r="AM58">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="AN58">
         <f t="shared" si="2"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -80226,11 +80694,19 @@
         <v>7</v>
       </c>
       <c r="AL59">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="AM59">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN59">
         <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -80329,11 +80805,19 @@
         <v>7</v>
       </c>
       <c r="AL60">
+        <f t="shared" si="4"/>
+        <v>-3</v>
+      </c>
+      <c r="AM60">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="AN60">
         <f t="shared" si="2"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -80414,11 +80898,19 @@
         <v>7</v>
       </c>
       <c r="AL61">
+        <f t="shared" si="4"/>
+        <v>-6</v>
+      </c>
+      <c r="AM61">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="AN61">
         <f t="shared" si="2"/>
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>106</v>
       </c>
@@ -80517,11 +81009,19 @@
         <v>5</v>
       </c>
       <c r="AL62">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM62">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN62">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>106</v>
       </c>
@@ -80626,11 +81126,19 @@
         <v>6</v>
       </c>
       <c r="AL63">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM63">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN63">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>106</v>
       </c>
@@ -80723,11 +81231,19 @@
         <v>6</v>
       </c>
       <c r="AL64">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="AM64">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN64">
         <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>106</v>
       </c>
@@ -80826,11 +81342,19 @@
         <v>5</v>
       </c>
       <c r="AL65">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM65">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AN65">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>59</v>
       </c>
@@ -80935,11 +81459,19 @@
         <v>6</v>
       </c>
       <c r="AL66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM66">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="AN66">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>59</v>
       </c>
@@ -81028,15 +81560,23 @@
         <v>1</v>
       </c>
       <c r="AK67">
-        <f t="shared" ref="AK67:AK90" si="3">SUM(O67,Q67,S67,U67,W67,Y67,AA67,AC67,AE67,AG67,AI67,2)</f>
+        <f t="shared" ref="AK67:AK90" si="5">SUM(O67,Q67,S67,U67,W67,Y67,AA67,AC67,AE67,AG67,AI67,2)</f>
         <v>7</v>
       </c>
       <c r="AL67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="68" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM67">
+        <f t="shared" ref="AM67:AM121" si="6">O67+Q67+S67+U67+W67+Y67+2</f>
+        <v>5</v>
+      </c>
+      <c r="AN67">
+        <f t="shared" ref="AN67:AN121" si="7">O67+S67+W67+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>59</v>
       </c>
@@ -81131,15 +81671,23 @@
         <v>0</v>
       </c>
       <c r="AK68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AL68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM68">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN68">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>59</v>
       </c>
@@ -81222,15 +81770,23 @@
         <v>0</v>
       </c>
       <c r="AK69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
-    </row>
-    <row r="70" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM69">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN69">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>60</v>
       </c>
@@ -81325,15 +81881,23 @@
         <v>0</v>
       </c>
       <c r="AK70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AL70">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM70">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN70">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>60</v>
       </c>
@@ -81437,15 +82001,23 @@
         <v>61</v>
       </c>
       <c r="AK71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL71">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM71">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN71">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>60</v>
       </c>
@@ -81534,15 +82106,23 @@
         <v>0</v>
       </c>
       <c r="AK72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM72">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN72">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>60</v>
       </c>
@@ -81643,15 +82223,23 @@
         <v>0</v>
       </c>
       <c r="AK73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL73">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM73">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN73">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>62</v>
       </c>
@@ -81752,15 +82340,23 @@
         <v>0</v>
       </c>
       <c r="AK74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL74">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM74">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN74">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>62</v>
       </c>
@@ -81849,15 +82445,23 @@
         <v>0</v>
       </c>
       <c r="AK75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="AL75">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AM75">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN75">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>62</v>
       </c>
@@ -81958,15 +82562,23 @@
         <v>0</v>
       </c>
       <c r="AK76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL76">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM76">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN76">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>62</v>
       </c>
@@ -82073,15 +82685,23 @@
         <v>0</v>
       </c>
       <c r="AK77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AL77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="78" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM77">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN77">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>63</v>
       </c>
@@ -82176,15 +82796,23 @@
         <v>0</v>
       </c>
       <c r="AK78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AL78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM78">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN78">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>63</v>
       </c>
@@ -82288,15 +82916,23 @@
         <v>64</v>
       </c>
       <c r="AK79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL79">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM79">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN79">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>63</v>
       </c>
@@ -82397,15 +83033,23 @@
         <v>0</v>
       </c>
       <c r="AK80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL80">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM80">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN80">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>63</v>
       </c>
@@ -82494,15 +83138,23 @@
         <v>0</v>
       </c>
       <c r="AK81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AL81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="82" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM81">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN81">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>65</v>
       </c>
@@ -82597,15 +83249,23 @@
         <v>0</v>
       </c>
       <c r="AK82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AL82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="83" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM82">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN82">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>65</v>
       </c>
@@ -82700,15 +83360,23 @@
         <v>0</v>
       </c>
       <c r="AK83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AL83">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM83">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN83">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>65</v>
       </c>
@@ -82803,15 +83471,23 @@
         <v>0</v>
       </c>
       <c r="AK84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL84">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM84">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN84">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>65</v>
       </c>
@@ -82894,15 +83570,23 @@
         <v>1</v>
       </c>
       <c r="AK85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AL85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
-    </row>
-    <row r="86" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM85">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN85">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>66</v>
       </c>
@@ -82991,15 +83675,23 @@
         <v>0</v>
       </c>
       <c r="AK86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="AL86">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AM86">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN86">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>66</v>
       </c>
@@ -83088,15 +83780,23 @@
         <v>1</v>
       </c>
       <c r="AK87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AL87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="88" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM87">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN87">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>66</v>
       </c>
@@ -83185,15 +83885,23 @@
         <v>1</v>
       </c>
       <c r="AK88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AL88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="89" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM88">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN88">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>66</v>
       </c>
@@ -83288,15 +83996,23 @@
         <v>0</v>
       </c>
       <c r="AK89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AL89">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM89">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN89">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>67</v>
       </c>
@@ -83373,15 +84089,23 @@
         <v>0</v>
       </c>
       <c r="AK90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AL90">
-        <f t="shared" ref="AL90:AL113" si="4">IF(K90&lt;&gt;0, K90-AK90,"")</f>
+        <f t="shared" ref="AL90:AL113" si="8">IF(K90&lt;&gt;0, K90-AK90,"")</f>
         <v>-4</v>
       </c>
-    </row>
-    <row r="91" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM90">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN90">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>67</v>
       </c>
@@ -83452,11 +84176,11 @@
         <v>68</v>
       </c>
       <c r="AL91" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>67</v>
       </c>
@@ -83533,15 +84257,23 @@
         <v>0</v>
       </c>
       <c r="AK92">
-        <f t="shared" ref="AK92:AK121" si="5">SUM(O92,Q92,S92,U92,W92,Y92,AA92,AC92,AE92,AG92,AI92,2)</f>
+        <f t="shared" ref="AK92:AK121" si="9">SUM(O92,Q92,S92,U92,W92,Y92,AA92,AC92,AE92,AG92,AI92,2)</f>
         <v>6</v>
       </c>
       <c r="AL92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="93" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM92">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN92">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>67</v>
       </c>
@@ -83618,11 +84350,11 @@
         <v>69</v>
       </c>
       <c r="AL93" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>70</v>
       </c>
@@ -83711,15 +84443,23 @@
         <v>0</v>
       </c>
       <c r="AK94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AL94">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="AM94">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="AN94">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>70</v>
       </c>
@@ -83814,15 +84554,23 @@
         <v>0</v>
       </c>
       <c r="AK95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AL95">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AM95">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN95">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>70</v>
       </c>
@@ -83917,15 +84665,23 @@
         <v>0</v>
       </c>
       <c r="AK96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AL96">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AM96">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN96">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>70</v>
       </c>
@@ -84008,15 +84764,23 @@
         <v>0</v>
       </c>
       <c r="AK97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AL97">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="AM97">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="AN97">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>71</v>
       </c>
@@ -84123,15 +84887,23 @@
         <v>0</v>
       </c>
       <c r="AK98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AL98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="99" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM98">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN98">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>71</v>
       </c>
@@ -84226,15 +84998,23 @@
         <v>1</v>
       </c>
       <c r="AK99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AL99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-5</v>
       </c>
-    </row>
-    <row r="100" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM99">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN99">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>71</v>
       </c>
@@ -84335,15 +85115,23 @@
         <v>0</v>
       </c>
       <c r="AK100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AL100">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AM100">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN100">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>71</v>
       </c>
@@ -84438,15 +85226,23 @@
         <v>0</v>
       </c>
       <c r="AK101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AL101">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AM101">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN101">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>72</v>
       </c>
@@ -84541,15 +85337,23 @@
         <v>0</v>
       </c>
       <c r="AK102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AL102">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AM102">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN102">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>72</v>
       </c>
@@ -84626,15 +85430,23 @@
         <v>0</v>
       </c>
       <c r="AK103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AL103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="104" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM103">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="AN103">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>72</v>
       </c>
@@ -84729,15 +85541,23 @@
         <v>0</v>
       </c>
       <c r="AK104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AL104">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AM104">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN104">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>72</v>
       </c>
@@ -84844,15 +85664,23 @@
         <v>0</v>
       </c>
       <c r="AK105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AL105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="106" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM105">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN105">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>73</v>
       </c>
@@ -84896,7 +85724,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="107" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>73</v>
       </c>
@@ -84964,7 +85792,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>73</v>
       </c>
@@ -84996,7 +85824,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="109" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>73</v>
       </c>
@@ -85025,7 +85853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>76</v>
       </c>
@@ -85126,15 +85954,23 @@
         <v>0</v>
       </c>
       <c r="AK110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AL110">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AM110">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN110">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>76</v>
       </c>
@@ -85229,15 +86065,23 @@
         <v>0</v>
       </c>
       <c r="AK111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AL111">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AM111">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN111">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>76</v>
       </c>
@@ -85338,15 +86182,23 @@
         <v>0</v>
       </c>
       <c r="AK112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AL112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM112">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AN112">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>76</v>
       </c>
@@ -85435,15 +86287,23 @@
         <v>0</v>
       </c>
       <c r="AK113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AL113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="114" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM113">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AN113">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>77</v>
       </c>
@@ -85475,7 +86335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>77</v>
       </c>
@@ -85507,7 +86367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>77</v>
       </c>
@@ -85539,7 +86399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>77</v>
       </c>
@@ -85571,7 +86431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>78</v>
       </c>
@@ -85654,15 +86514,23 @@
         <v>1</v>
       </c>
       <c r="AK118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AL118">
-        <f t="shared" ref="AL118:AL121" si="6">IF(K118&lt;&gt;0, K118-AK118,"")</f>
+        <f t="shared" ref="AL118:AL121" si="10">IF(K118&lt;&gt;0, K118-AK118,"")</f>
         <v>-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AM118">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AN118">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>78</v>
       </c>
@@ -85757,15 +86625,23 @@
         <v>0</v>
       </c>
       <c r="AK119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AL119">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AM119">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AN119">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>78</v>
       </c>
@@ -85866,15 +86742,23 @@
         <v>0</v>
       </c>
       <c r="AK120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AL120">
+        <f t="shared" si="10"/>
+        <v>-2</v>
+      </c>
+      <c r="AM120">
         <f t="shared" si="6"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AN120">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>78</v>
       </c>
@@ -85975,12 +86859,20 @@
         <v>0</v>
       </c>
       <c r="AK121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AL121">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AM121">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="AN121">
+        <f t="shared" si="7"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move the data files to another folder
correction of mistake in the calculation of the difference score in the test files
</commit_message>
<xml_diff>
--- a/data/20181122 WM tasks.xlsx
+++ b/data/20181122 WM tasks.xlsx
@@ -74256,10 +74256,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="AM26" sqref="AM26"/>
+      <selection pane="bottomLeft" activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74495,7 +74495,7 @@
         <v>5</v>
       </c>
       <c r="AL2">
-        <f>IF(K2&lt;&gt;0, K2-AK2,"")</f>
+        <f>IF(K2&lt;&gt;"", K2-AK2,"")</f>
         <v>1</v>
       </c>
       <c r="AM2">
@@ -74612,15 +74612,15 @@
         <v>6</v>
       </c>
       <c r="AL3">
-        <f>IF(K3&lt;&gt;0, K3-AK3,"")</f>
+        <f t="shared" ref="AL3:AL66" si="1">IF(K3&lt;&gt;"", K3-AK3,"")</f>
         <v>0</v>
       </c>
       <c r="AM3">
-        <f t="shared" ref="AM3:AM66" si="1">O3+Q3+S3+U3+W3+Y3+2</f>
+        <f t="shared" ref="AM3:AM66" si="2">O3+Q3+S3+U3+W3+Y3+2</f>
         <v>4</v>
       </c>
       <c r="AN3">
-        <f t="shared" ref="AN3:AN66" si="2">O3+S3+W3+1</f>
+        <f t="shared" ref="AN3:AN66" si="3">O3+S3+W3+1</f>
         <v>2</v>
       </c>
     </row>
@@ -74729,15 +74729,15 @@
         <v>6</v>
       </c>
       <c r="AL4">
-        <f t="shared" ref="AL4:AL43" si="3">IF(K4&lt;&gt;0, K4-AK4,"")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -74822,15 +74822,15 @@
         <v>7</v>
       </c>
       <c r="AL5">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="AN5">
         <f t="shared" si="3"/>
-        <v>-6</v>
-      </c>
-      <c r="AM5">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="AN5">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -74939,15 +74939,15 @@
         <v>6</v>
       </c>
       <c r="AL6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN6">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN6">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -75050,15 +75050,15 @@
         <v>7</v>
       </c>
       <c r="AL7">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN7">
         <f t="shared" si="3"/>
-        <v>-3</v>
-      </c>
-      <c r="AM7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN7">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -75167,15 +75167,15 @@
         <v>7</v>
       </c>
       <c r="AL8">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN8">
         <f t="shared" si="3"/>
-        <v>-2</v>
-      </c>
-      <c r="AM8">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN8">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -75261,15 +75261,15 @@
         <v>7</v>
       </c>
       <c r="AL9">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="AN9">
         <f t="shared" si="3"/>
-        <v>-6</v>
-      </c>
-      <c r="AM9">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="AN9">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -75366,15 +75366,15 @@
         <v>8</v>
       </c>
       <c r="AL10">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN10">
         <f t="shared" si="3"/>
-        <v>-6</v>
-      </c>
-      <c r="AM10">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN10">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -75483,15 +75483,15 @@
         <v>6</v>
       </c>
       <c r="AL11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN11">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AM11">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN11">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -75597,15 +75597,15 @@
         <v>6</v>
       </c>
       <c r="AL12">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN12">
         <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="AM12">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN12">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -75708,15 +75708,15 @@
         <v>5</v>
       </c>
       <c r="AL13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN13">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM13">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN13">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -75807,15 +75807,15 @@
         <v>4</v>
       </c>
       <c r="AL14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM14">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN14">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM14">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN14">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -75924,15 +75924,15 @@
         <v>7</v>
       </c>
       <c r="AL15">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="AM15">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN15">
         <f t="shared" si="3"/>
-        <v>-2</v>
-      </c>
-      <c r="AM15">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN15">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -76017,15 +76017,15 @@
         <v>5</v>
       </c>
       <c r="AL16">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="AM16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN16">
         <f t="shared" si="3"/>
-        <v>-2</v>
-      </c>
-      <c r="AM16">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN16">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -76128,15 +76128,15 @@
         <v>5</v>
       </c>
       <c r="AL17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM17">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN17">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM17">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN17">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -76227,15 +76227,15 @@
         <v>7</v>
       </c>
       <c r="AL18">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN18">
         <f t="shared" si="3"/>
-        <v>-5</v>
-      </c>
-      <c r="AM18">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN18">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -76344,15 +76344,15 @@
         <v>6</v>
       </c>
       <c r="AL19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM19">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AM19">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN19">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -76461,15 +76461,15 @@
         <v>8</v>
       </c>
       <c r="AL20">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN20">
         <f t="shared" si="3"/>
-        <v>-4</v>
-      </c>
-      <c r="AM20">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN20">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -76578,15 +76578,15 @@
         <v>6</v>
       </c>
       <c r="AL21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM21">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN21">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AM21">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN21">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -76683,15 +76683,15 @@
         <v>4</v>
       </c>
       <c r="AL22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AM22">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN22">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="AM22">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN22">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -76788,15 +76788,15 @@
         <v>4</v>
       </c>
       <c r="AL23">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AM23">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN23">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="AM23">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN23">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -76899,15 +76899,15 @@
         <v>5</v>
       </c>
       <c r="AL24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM24">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN24">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM24">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN24">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -77010,15 +77010,15 @@
         <v>6</v>
       </c>
       <c r="AL25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM25">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN25">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AM25">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN25">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -77115,15 +77115,15 @@
         <v>4</v>
       </c>
       <c r="AL26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AM26">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AN26">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="AM26">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="AN26">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -77214,15 +77214,15 @@
         <v>3</v>
       </c>
       <c r="AL27">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AM27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AN27">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="AM27">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="AN27">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -77313,15 +77313,15 @@
         <v>3</v>
       </c>
       <c r="AL28">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AM28">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AN28">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="AM28">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="AN28">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -77412,15 +77412,15 @@
         <v>3</v>
       </c>
       <c r="AL29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AM29">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="AN29">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="AM29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="AN29">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -77523,15 +77523,15 @@
         <v>5</v>
       </c>
       <c r="AL30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM30">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN30">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM30">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN30">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -77634,15 +77634,15 @@
         <v>5</v>
       </c>
       <c r="AL31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM31">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN31">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM31">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN31">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -77739,15 +77739,15 @@
         <v>4</v>
       </c>
       <c r="AL32">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AM32">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN32">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="AM32">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN32">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -77850,15 +77850,15 @@
         <v>5</v>
       </c>
       <c r="AL33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM33">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN33">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM33">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN33">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -77955,15 +77955,15 @@
         <v>7</v>
       </c>
       <c r="AL34">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="AM34">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN34">
         <f t="shared" si="3"/>
-        <v>-4</v>
-      </c>
-      <c r="AM34">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN34">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -78060,15 +78060,15 @@
         <v>5</v>
       </c>
       <c r="AL35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM35">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN35">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM35">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN35">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -78177,15 +78177,15 @@
         <v>6</v>
       </c>
       <c r="AL36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM36">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN36">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AM36">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN36">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -78270,15 +78270,15 @@
         <v>6</v>
       </c>
       <c r="AL37">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="AM37">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN37">
         <f t="shared" si="3"/>
-        <v>-4</v>
-      </c>
-      <c r="AM37">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN37">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -78369,15 +78369,15 @@
         <v>7</v>
       </c>
       <c r="AL38">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="AM38">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="AN38">
         <f t="shared" si="3"/>
-        <v>-4</v>
-      </c>
-      <c r="AM38">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="AN38">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -78474,15 +78474,15 @@
         <v>6</v>
       </c>
       <c r="AL39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM39">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN39">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AM39">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN39">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -78585,15 +78585,15 @@
         <v>5</v>
       </c>
       <c r="AL40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM40">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN40">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM40">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN40">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -78690,15 +78690,15 @@
         <v>4</v>
       </c>
       <c r="AL41">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="AM41">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AN41">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="AM41">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="AN41">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -78813,15 +78813,15 @@
         <v>8</v>
       </c>
       <c r="AL42">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="AM42">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN42">
         <f t="shared" si="3"/>
-        <v>-4</v>
-      </c>
-      <c r="AM42">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN42">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -78924,15 +78924,15 @@
         <v>5</v>
       </c>
       <c r="AL43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AM43">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AN43">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AM43">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="AN43">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -79041,15 +79041,15 @@
         <v>5</v>
       </c>
       <c r="AL44">
-        <f t="shared" ref="AL44:AL89" si="4">IF(K44&lt;&gt;0, K44-AK44,"")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AM44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -79146,15 +79146,15 @@
         <v>4</v>
       </c>
       <c r="AL45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AM45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -79263,15 +79263,15 @@
         <v>6</v>
       </c>
       <c r="AL46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -79374,15 +79374,15 @@
         <v>6</v>
       </c>
       <c r="AL47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -79485,15 +79485,15 @@
         <v>5</v>
       </c>
       <c r="AL48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AM48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -79596,15 +79596,15 @@
         <v>5</v>
       </c>
       <c r="AL49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AM49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -79707,15 +79707,15 @@
         <v>5</v>
       </c>
       <c r="AL50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AM50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -79806,15 +79806,15 @@
         <v>6</v>
       </c>
       <c r="AL51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="AM51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AN51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -79923,15 +79923,15 @@
         <v>6</v>
       </c>
       <c r="AL52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -80034,15 +80034,15 @@
         <v>5</v>
       </c>
       <c r="AL53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AM53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -80139,15 +80139,15 @@
         <v>4</v>
       </c>
       <c r="AL54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AM54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -80244,15 +80244,15 @@
         <v>4</v>
       </c>
       <c r="AL55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AM55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AN55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -80349,15 +80349,15 @@
         <v>4</v>
       </c>
       <c r="AL56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AM56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -80460,15 +80460,15 @@
         <v>5</v>
       </c>
       <c r="AL57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AM57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AN57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -80577,15 +80577,15 @@
         <v>8</v>
       </c>
       <c r="AL58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
       <c r="AM58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AN58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -80694,15 +80694,15 @@
         <v>7</v>
       </c>
       <c r="AL59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="AM59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -80805,15 +80805,15 @@
         <v>7</v>
       </c>
       <c r="AL60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="AM60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AN60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -80898,15 +80898,15 @@
         <v>7</v>
       </c>
       <c r="AL61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
       <c r="AM61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="AN61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -81009,15 +81009,15 @@
         <v>5</v>
       </c>
       <c r="AL62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AM62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -81126,15 +81126,15 @@
         <v>6</v>
       </c>
       <c r="AL63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -81231,15 +81231,15 @@
         <v>6</v>
       </c>
       <c r="AL64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="AM64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -81342,15 +81342,15 @@
         <v>5</v>
       </c>
       <c r="AL65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AM65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AN65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -81459,15 +81459,15 @@
         <v>6</v>
       </c>
       <c r="AL66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AN66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -81560,11 +81560,11 @@
         <v>1</v>
       </c>
       <c r="AK67">
-        <f t="shared" ref="AK67:AK90" si="5">SUM(O67,Q67,S67,U67,W67,Y67,AA67,AC67,AE67,AG67,AI67,2)</f>
+        <f t="shared" ref="AK67:AK90" si="4">SUM(O67,Q67,S67,U67,W67,Y67,AA67,AC67,AE67,AG67,AI67,2)</f>
         <v>7</v>
       </c>
       <c r="AL67">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AL67:AL105" si="5">IF(K67&lt;&gt;"", K67-AK67,"")</f>
         <v>-4</v>
       </c>
       <c r="AM67">
@@ -81671,11 +81671,11 @@
         <v>0</v>
       </c>
       <c r="AK68">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL68">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AL68">
-        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
       <c r="AM68">
@@ -81770,11 +81770,11 @@
         <v>0</v>
       </c>
       <c r="AK69">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL69">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL69">
-        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
       <c r="AM69">
@@ -81881,11 +81881,11 @@
         <v>0</v>
       </c>
       <c r="AK70">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AL70">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="AL70">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AM70">
@@ -82001,11 +82001,11 @@
         <v>61</v>
       </c>
       <c r="AK71">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL71">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL71">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM71">
@@ -82106,11 +82106,11 @@
         <v>0</v>
       </c>
       <c r="AK72">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL72">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL72">
-        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="AM72">
@@ -82223,11 +82223,11 @@
         <v>0</v>
       </c>
       <c r="AK73">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL73">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL73">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM73">
@@ -82340,11 +82340,11 @@
         <v>0</v>
       </c>
       <c r="AK74">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL74">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL74">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM74">
@@ -82445,11 +82445,11 @@
         <v>0</v>
       </c>
       <c r="AK75">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AL75">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="AL75">
-        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AM75">
@@ -82562,11 +82562,11 @@
         <v>0</v>
       </c>
       <c r="AK76">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL76">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL76">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM76">
@@ -82685,11 +82685,11 @@
         <v>0</v>
       </c>
       <c r="AK77">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL77">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AL77">
-        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="AM77">
@@ -82796,11 +82796,11 @@
         <v>0</v>
       </c>
       <c r="AK78">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL78">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AL78">
-        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
       <c r="AM78">
@@ -82916,11 +82916,11 @@
         <v>64</v>
       </c>
       <c r="AK79">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL79">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL79">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM79">
@@ -83033,11 +83033,11 @@
         <v>0</v>
       </c>
       <c r="AK80">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL80">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL80">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM80">
@@ -83138,11 +83138,11 @@
         <v>0</v>
       </c>
       <c r="AK81">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL81">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AL81">
-        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
       <c r="AM81">
@@ -83249,11 +83249,11 @@
         <v>0</v>
       </c>
       <c r="AK82">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL82">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AL82">
-        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
       <c r="AM82">
@@ -83360,11 +83360,11 @@
         <v>0</v>
       </c>
       <c r="AK83">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AL83">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="AL83">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AM83">
@@ -83471,11 +83471,11 @@
         <v>0</v>
       </c>
       <c r="AK84">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL84">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL84">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM84">
@@ -83570,11 +83570,11 @@
         <v>1</v>
       </c>
       <c r="AK85">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL85">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AL85">
-        <f t="shared" si="4"/>
         <v>-5</v>
       </c>
       <c r="AM85">
@@ -83675,11 +83675,11 @@
         <v>0</v>
       </c>
       <c r="AK86">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AL86">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="AL86">
-        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AM86">
@@ -83780,11 +83780,11 @@
         <v>1</v>
       </c>
       <c r="AK87">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL87">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AL87">
-        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
       <c r="AM87">
@@ -83885,11 +83885,11 @@
         <v>1</v>
       </c>
       <c r="AK88">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL88">
         <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AL88">
-        <f t="shared" si="4"/>
         <v>-4</v>
       </c>
       <c r="AM88">
@@ -83996,11 +83996,11 @@
         <v>0</v>
       </c>
       <c r="AK89">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AL89">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="AL89">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AM89">
@@ -84089,11 +84089,11 @@
         <v>0</v>
       </c>
       <c r="AK90">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AL90">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL90">
-        <f t="shared" ref="AL90:AL113" si="8">IF(K90&lt;&gt;0, K90-AK90,"")</f>
         <v>-4</v>
       </c>
       <c r="AM90">
@@ -84176,7 +84176,7 @@
         <v>68</v>
       </c>
       <c r="AL91" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -84257,11 +84257,11 @@
         <v>0</v>
       </c>
       <c r="AK92">
-        <f t="shared" ref="AK92:AK121" si="9">SUM(O92,Q92,S92,U92,W92,Y92,AA92,AC92,AE92,AG92,AI92,2)</f>
+        <f t="shared" ref="AK92:AK121" si="8">SUM(O92,Q92,S92,U92,W92,Y92,AA92,AC92,AE92,AG92,AI92,2)</f>
         <v>6</v>
       </c>
       <c r="AL92">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>-4</v>
       </c>
       <c r="AM92">
@@ -84350,7 +84350,7 @@
         <v>69</v>
       </c>
       <c r="AL93" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -84443,11 +84443,11 @@
         <v>0</v>
       </c>
       <c r="AK94">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AL94">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="AM94">
@@ -84554,11 +84554,11 @@
         <v>0</v>
       </c>
       <c r="AK95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AL95">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AM95">
@@ -84665,11 +84665,11 @@
         <v>0</v>
       </c>
       <c r="AK96">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AL96">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AM96">
@@ -84764,11 +84764,11 @@
         <v>0</v>
       </c>
       <c r="AK97">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="AL97">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="AM97">
@@ -84887,11 +84887,11 @@
         <v>0</v>
       </c>
       <c r="AK98">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AL98">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="AM98">
@@ -84998,11 +84998,11 @@
         <v>1</v>
       </c>
       <c r="AK99">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="AL99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>-5</v>
       </c>
       <c r="AM99">
@@ -85115,11 +85115,11 @@
         <v>0</v>
       </c>
       <c r="AK100">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="AL100">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AM100">
@@ -85226,11 +85226,11 @@
         <v>0</v>
       </c>
       <c r="AK101">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AL101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AM101">
@@ -85337,11 +85337,11 @@
         <v>0</v>
       </c>
       <c r="AK102">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AL102">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AM102">
@@ -85430,11 +85430,11 @@
         <v>0</v>
       </c>
       <c r="AK103">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AL103">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>-6</v>
       </c>
       <c r="AM103">
@@ -85541,11 +85541,11 @@
         <v>0</v>
       </c>
       <c r="AK104">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="AL104">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AM104">
@@ -85664,11 +85664,11 @@
         <v>0</v>
       </c>
       <c r="AK105">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="AL105">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="AM105">
@@ -85723,6 +85723,10 @@
       <c r="AJ106" t="s">
         <v>74</v>
       </c>
+      <c r="AL106" t="str">
+        <f>IF(K106&lt;&gt;"", K106-AK106,"")</f>
+        <v/>
+      </c>
     </row>
     <row r="107" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
@@ -85791,6 +85795,10 @@
       <c r="AJ107" t="s">
         <v>74</v>
       </c>
+      <c r="AL107" t="str">
+        <f t="shared" ref="AL107:AL121" si="9">IF(K107&lt;&gt;"", K107-AK107,"")</f>
+        <v/>
+      </c>
     </row>
     <row r="108" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
@@ -85823,6 +85831,10 @@
       <c r="AJ108" t="s">
         <v>75</v>
       </c>
+      <c r="AL108" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
     </row>
     <row r="109" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
@@ -85852,6 +85864,10 @@
       <c r="I109">
         <v>4</v>
       </c>
+      <c r="AL109" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
     </row>
     <row r="110" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
@@ -85954,11 +85970,11 @@
         <v>0</v>
       </c>
       <c r="AK110">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AL110">
         <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
-      <c r="AL110">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AM110">
@@ -86065,11 +86081,11 @@
         <v>0</v>
       </c>
       <c r="AK111">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AL111">
         <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="AL111">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="AM111">
@@ -86182,11 +86198,11 @@
         <v>0</v>
       </c>
       <c r="AK112">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AL112">
         <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="AL112">
-        <f t="shared" si="8"/>
         <v>-2</v>
       </c>
       <c r="AM112">
@@ -86287,11 +86303,11 @@
         <v>0</v>
       </c>
       <c r="AK113">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AL113">
         <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="AL113">
-        <f t="shared" si="8"/>
         <v>-4</v>
       </c>
       <c r="AM113">
@@ -86334,6 +86350,10 @@
       <c r="J114">
         <v>0</v>
       </c>
+      <c r="AL114" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
     </row>
     <row r="115" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
@@ -86366,6 +86386,10 @@
       <c r="J115">
         <v>0</v>
       </c>
+      <c r="AL115" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
     </row>
     <row r="116" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
@@ -86398,6 +86422,10 @@
       <c r="J116">
         <v>0</v>
       </c>
+      <c r="AL116" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
     </row>
     <row r="117" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
@@ -86430,6 +86458,10 @@
       <c r="J117">
         <v>0</v>
       </c>
+      <c r="AL117" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
     </row>
     <row r="118" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
@@ -86514,11 +86546,11 @@
         <v>1</v>
       </c>
       <c r="AK118">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AL118">
         <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
-      <c r="AL118">
-        <f t="shared" ref="AL118:AL121" si="10">IF(K118&lt;&gt;0, K118-AK118,"")</f>
         <v>-3</v>
       </c>
       <c r="AM118">
@@ -86625,11 +86657,11 @@
         <v>0</v>
       </c>
       <c r="AK119">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AL119">
         <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="AL119">
-        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AM119">
@@ -86742,11 +86774,11 @@
         <v>0</v>
       </c>
       <c r="AK120">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AL120">
         <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="AL120">
-        <f t="shared" si="10"/>
         <v>-2</v>
       </c>
       <c r="AM120">
@@ -86859,11 +86891,11 @@
         <v>0</v>
       </c>
       <c r="AK121">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AL121">
         <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
-      <c r="AL121">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AM121">

</xml_diff>